<commit_message>
Ula: changes in parser
</commit_message>
<xml_diff>
--- a/EXCEL.xlsx
+++ b/EXCEL.xlsx
@@ -11,27 +11,86 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>deposit</t>
-  </si>
-  <si>
-    <t>account</t>
-  </si>
-  <si>
-    <t>name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+  <si>
+    <t>Bet</t>
+  </si>
+  <si>
+    <t>Total_Strake</t>
+  </si>
+  <si>
+    <t>Benefit</t>
+  </si>
+  <si>
+    <t>Odds</t>
+  </si>
+  <si>
+    <t>Express</t>
+  </si>
+  <si>
+    <t>Atl Mdr-Barca 2 team win or draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Man C-Man U 2 team win or draw</t>
+  </si>
+  <si>
+    <t>Troynik</t>
+  </si>
+  <si>
+    <t>Bor Dor-Bayern 1 team win or draw</t>
+  </si>
+  <si>
+    <t>CSKA-Roma 2 team win</t>
+  </si>
+  <si>
+    <t>Kabrera-Yuan 1  win</t>
+  </si>
+  <si>
+    <t>Kabrera-Yuan 2 win</t>
+  </si>
+  <si>
+    <t>Spartak - Ural 2 team win</t>
+  </si>
+  <si>
+    <t>Kraynik - Videnmann 1 win</t>
+  </si>
+  <si>
+    <t>Kraynik - Videnmann 1 win 2 set</t>
+  </si>
+  <si>
+    <t>Etcheverri- Collarini 2 win set 3</t>
+  </si>
+  <si>
+    <t>Etcheverri- Collarini 1 win set 3</t>
+  </si>
+  <si>
+    <t>Clasen/Venus-Royer/Tekau 2 team win</t>
+  </si>
+  <si>
+    <t>Sok-Tim 1 win set 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="#&quot; &quot;?/10"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,14 +116,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -363,60 +435,429 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="12" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6">
+        <v>100</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2.79</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="B3" s="3">
+        <v>78</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1.41</v>
+      </c>
+      <c r="D3" s="5">
+        <v>109.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>69</v>
+      </c>
+      <c r="C4" s="5">
+        <v>16.21</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>100</v>
+      </c>
+      <c r="C5" s="5">
+        <v>9.26</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B6" s="3">
+        <v>70</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>100</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D7" s="5">
+        <v>247.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>100</v>
+      </c>
+      <c r="C8" s="5">
+        <v>3.18</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2.23</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3">
+        <v>100</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2.15</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3">
+        <v>100</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3.27</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
+      <c r="B12" s="3">
+        <v>100</v>
+      </c>
+      <c r="C12" s="5">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D12" s="5">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3">
+        <v>100</v>
+      </c>
+      <c r="C13" s="5">
+        <v>5.14</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <v>100</v>
+      </c>
+      <c r="C14" s="5">
+        <v>7.29</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3">
+        <v>50</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1.71</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3">
+        <v>50</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2.02</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3">
+        <v>100</v>
+      </c>
+      <c r="C17" s="5">
+        <v>2.9</v>
+      </c>
+      <c r="D17" s="5">
+        <v>290.16000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3">
+        <v>100</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1.92</v>
+      </c>
+      <c r="D18" s="5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="3">
+        <v>50</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="D19" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="3">
+        <v>50</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="D20" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="3">
+        <v>50</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1.32</v>
+      </c>
+      <c r="D21" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="3">
+        <v>50</v>
+      </c>
+      <c r="C22" s="5">
+        <v>1.75</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3">
+        <v>113</v>
+      </c>
+      <c r="C23" s="5">
+        <v>3.19</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3">
+        <v>100</v>
+      </c>
+      <c r="C24" s="5">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3">
+        <v>100</v>
+      </c>
+      <c r="C25" s="5">
+        <v>10.46</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="3">
+        <v>100</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D26" s="5">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="3">
+        <v>46</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1.62</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>